<commit_message>
Update reference file: Y5_B2425_Pediatrics_reference_data.xlsx
</commit_message>
<xml_diff>
--- a/reference_data/Y5_B2425_Pediatrics_reference_data.xlsx
+++ b/reference_data/Y5_B2425_Pediatrics_reference_data.xlsx
@@ -479,7 +479,7 @@
     <col width="46" customWidth="1" min="2" max="2"/>
     <col width="8" customWidth="1" min="3" max="3"/>
     <col width="10" customWidth="1" min="4" max="4"/>
-    <col width="38" customWidth="1" min="5" max="5"/>
+    <col width="42" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -532,7 +532,7 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -559,7 +559,7 @@
       </c>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -586,7 +586,7 @@
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -613,7 +613,7 @@
       </c>
       <c r="E5" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -640,7 +640,7 @@
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -694,7 +694,7 @@
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -721,7 +721,7 @@
       </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -748,7 +748,7 @@
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -775,7 +775,7 @@
       </c>
       <c r="E11" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -802,7 +802,7 @@
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -829,7 +829,7 @@
       </c>
       <c r="E13" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -856,7 +856,7 @@
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -883,7 +883,7 @@
       </c>
       <c r="E15" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -910,7 +910,7 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -937,7 +937,7 @@
       </c>
       <c r="E17" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -964,7 +964,7 @@
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -991,7 +991,7 @@
       </c>
       <c r="E19" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1018,7 +1018,7 @@
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="E21" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1072,7 +1072,7 @@
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1099,7 +1099,7 @@
       </c>
       <c r="E23" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1126,7 +1126,7 @@
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
       </c>
       <c r="E25" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1207,7 +1207,7 @@
       </c>
       <c r="E27" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1234,7 +1234,7 @@
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1261,7 +1261,7 @@
       </c>
       <c r="E29" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1315,7 +1315,7 @@
       </c>
       <c r="E31" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1369,7 +1369,7 @@
       </c>
       <c r="E33" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="E35" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1450,7 +1450,7 @@
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="E37" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1531,7 +1531,7 @@
       </c>
       <c r="E39" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1558,7 +1558,7 @@
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="E41" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1612,7 +1612,7 @@
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1639,7 +1639,7 @@
       </c>
       <c r="E43" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1666,7 +1666,7 @@
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1693,7 +1693,7 @@
       </c>
       <c r="E45" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="E47" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1774,7 +1774,7 @@
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1801,7 +1801,7 @@
       </c>
       <c r="E49" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1828,7 +1828,7 @@
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1855,7 +1855,7 @@
       </c>
       <c r="E51" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1882,7 +1882,7 @@
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1909,7 +1909,7 @@
       </c>
       <c r="E53" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1963,7 +1963,7 @@
       </c>
       <c r="E55" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -1990,7 +1990,7 @@
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2017,7 +2017,7 @@
       </c>
       <c r="E57" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2044,7 +2044,7 @@
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2071,7 +2071,7 @@
       </c>
       <c r="E59" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2098,7 +2098,7 @@
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="E61" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="E63" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2206,7 +2206,7 @@
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="E65" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2260,7 +2260,7 @@
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2287,7 +2287,7 @@
       </c>
       <c r="E67" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="E69" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2368,7 +2368,7 @@
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2395,7 +2395,7 @@
       </c>
       <c r="E71" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2422,7 +2422,7 @@
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2449,7 +2449,7 @@
       </c>
       <c r="E73" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2503,7 +2503,7 @@
       </c>
       <c r="E75" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2530,7 +2530,7 @@
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="E77" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2584,7 +2584,7 @@
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2611,7 +2611,7 @@
       </c>
       <c r="E79" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2665,7 +2665,7 @@
       </c>
       <c r="E81" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2692,7 +2692,7 @@
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2719,7 +2719,7 @@
       </c>
       <c r="E83" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2746,7 +2746,7 @@
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2773,7 +2773,7 @@
       </c>
       <c r="E85" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2800,7 +2800,7 @@
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2827,7 +2827,7 @@
       </c>
       <c r="E87" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2854,7 +2854,7 @@
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2881,7 +2881,7 @@
       </c>
       <c r="E89" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2935,7 +2935,7 @@
       </c>
       <c r="E91" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2962,7 +2962,7 @@
       </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -2989,7 +2989,7 @@
       </c>
       <c r="E93" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3016,7 +3016,7 @@
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3043,7 +3043,7 @@
       </c>
       <c r="E95" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3070,7 +3070,7 @@
       </c>
       <c r="E96" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3097,7 +3097,7 @@
       </c>
       <c r="E97" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3124,7 +3124,7 @@
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3151,7 +3151,7 @@
       </c>
       <c r="E99" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3178,7 +3178,7 @@
       </c>
       <c r="E100" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3205,7 +3205,7 @@
       </c>
       <c r="E101" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3232,7 +3232,7 @@
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3259,7 +3259,7 @@
       </c>
       <c r="E103" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3286,7 +3286,7 @@
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3313,7 +3313,7 @@
       </c>
       <c r="E105" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3340,7 +3340,7 @@
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3367,7 +3367,7 @@
       </c>
       <c r="E107" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3394,7 +3394,7 @@
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="E109" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3448,7 +3448,7 @@
       </c>
       <c r="E110" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3475,7 +3475,7 @@
       </c>
       <c r="E111" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3502,7 +3502,7 @@
       </c>
       <c r="E112" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="E113" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3556,7 +3556,7 @@
       </c>
       <c r="E114" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3583,7 +3583,7 @@
       </c>
       <c r="E115" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3610,7 +3610,7 @@
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3637,7 +3637,7 @@
       </c>
       <c r="E117" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3664,7 +3664,7 @@
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3691,7 +3691,7 @@
       </c>
       <c r="E119" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3718,7 +3718,7 @@
       </c>
       <c r="E120" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3745,7 +3745,7 @@
       </c>
       <c r="E121" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3772,7 +3772,7 @@
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3799,7 +3799,7 @@
       </c>
       <c r="E123" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3826,7 +3826,7 @@
       </c>
       <c r="E124" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3853,7 +3853,7 @@
       </c>
       <c r="E125" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3880,7 +3880,7 @@
       </c>
       <c r="E126" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3907,7 +3907,7 @@
       </c>
       <c r="E127" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3934,7 +3934,7 @@
       </c>
       <c r="E128" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3961,7 +3961,7 @@
       </c>
       <c r="E129" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="E130" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4015,7 +4015,7 @@
       </c>
       <c r="E131" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4042,7 +4042,7 @@
       </c>
       <c r="E132" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4069,7 +4069,7 @@
       </c>
       <c r="E133" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="E134" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4123,7 +4123,7 @@
       </c>
       <c r="E135" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4150,7 +4150,7 @@
       </c>
       <c r="E136" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4177,7 +4177,7 @@
       </c>
       <c r="E137" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4204,7 +4204,7 @@
       </c>
       <c r="E138" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4231,7 +4231,7 @@
       </c>
       <c r="E139" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="E140" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4285,7 +4285,7 @@
       </c>
       <c r="E141" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4312,7 +4312,7 @@
       </c>
       <c r="E142" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4339,7 +4339,7 @@
       </c>
       <c r="E143" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4366,7 +4366,7 @@
       </c>
       <c r="E144" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4393,7 +4393,7 @@
       </c>
       <c r="E145" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4420,7 +4420,7 @@
       </c>
       <c r="E146" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4447,7 +4447,7 @@
       </c>
       <c r="E147" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4474,7 +4474,7 @@
       </c>
       <c r="E148" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4501,7 +4501,7 @@
       </c>
       <c r="E149" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4528,7 +4528,7 @@
       </c>
       <c r="E150" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4555,7 +4555,7 @@
       </c>
       <c r="E151" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4582,7 +4582,7 @@
       </c>
       <c r="E152" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4609,7 +4609,7 @@
       </c>
       <c r="E153" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4636,7 +4636,7 @@
       </c>
       <c r="E154" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4663,7 +4663,7 @@
       </c>
       <c r="E155" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4690,7 +4690,7 @@
       </c>
       <c r="E156" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4717,7 +4717,7 @@
       </c>
       <c r="E157" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4744,7 +4744,7 @@
       </c>
       <c r="E158" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4771,7 +4771,7 @@
       </c>
       <c r="E159" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4798,7 +4798,7 @@
       </c>
       <c r="E160" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4825,7 +4825,7 @@
       </c>
       <c r="E161" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4852,7 +4852,7 @@
       </c>
       <c r="E162" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4879,7 +4879,7 @@
       </c>
       <c r="E163" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4906,7 +4906,7 @@
       </c>
       <c r="E164" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4933,7 +4933,7 @@
       </c>
       <c r="E165" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4960,7 +4960,7 @@
       </c>
       <c r="E166" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -4987,7 +4987,7 @@
       </c>
       <c r="E167" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5014,7 +5014,7 @@
       </c>
       <c r="E168" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5041,7 +5041,7 @@
       </c>
       <c r="E169" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5068,7 +5068,7 @@
       </c>
       <c r="E170" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5095,7 +5095,7 @@
       </c>
       <c r="E171" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5122,7 +5122,7 @@
       </c>
       <c r="E172" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5149,7 +5149,7 @@
       </c>
       <c r="E173" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5176,7 +5176,7 @@
       </c>
       <c r="E174" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="E175" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5230,7 +5230,7 @@
       </c>
       <c r="E176" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5257,7 +5257,7 @@
       </c>
       <c r="E177" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5284,7 +5284,7 @@
       </c>
       <c r="E178" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5311,7 +5311,7 @@
       </c>
       <c r="E179" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5338,7 +5338,7 @@
       </c>
       <c r="E180" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5365,7 +5365,7 @@
       </c>
       <c r="E181" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5392,7 +5392,7 @@
       </c>
       <c r="E182" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5419,7 +5419,7 @@
       </c>
       <c r="E183" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5446,7 +5446,7 @@
       </c>
       <c r="E184" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5473,7 +5473,7 @@
       </c>
       <c r="E185" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5500,7 +5500,7 @@
       </c>
       <c r="E186" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5527,7 +5527,7 @@
       </c>
       <c r="E187" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5554,7 +5554,7 @@
       </c>
       <c r="E188" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5581,7 +5581,7 @@
       </c>
       <c r="E189" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5608,7 +5608,7 @@
       </c>
       <c r="E190" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5635,7 +5635,7 @@
       </c>
       <c r="E191" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5662,7 +5662,7 @@
       </c>
       <c r="E192" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5689,7 +5689,7 @@
       </c>
       <c r="E193" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5716,7 +5716,7 @@
       </c>
       <c r="E194" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5743,7 +5743,7 @@
       </c>
       <c r="E195" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5770,7 +5770,7 @@
       </c>
       <c r="E196" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5797,7 +5797,7 @@
       </c>
       <c r="E197" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5824,7 +5824,7 @@
       </c>
       <c r="E198" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5851,7 +5851,7 @@
       </c>
       <c r="E199" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5878,7 +5878,7 @@
       </c>
       <c r="E200" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5905,7 +5905,7 @@
       </c>
       <c r="E201" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5932,7 +5932,7 @@
       </c>
       <c r="E202" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5959,7 +5959,7 @@
       </c>
       <c r="E203" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -5986,7 +5986,7 @@
       </c>
       <c r="E204" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6013,7 +6013,7 @@
       </c>
       <c r="E205" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6040,7 +6040,7 @@
       </c>
       <c r="E206" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6067,7 +6067,7 @@
       </c>
       <c r="E207" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6094,7 +6094,7 @@
       </c>
       <c r="E208" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6121,7 +6121,7 @@
       </c>
       <c r="E209" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6148,7 +6148,7 @@
       </c>
       <c r="E210" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6175,7 +6175,7 @@
       </c>
       <c r="E211" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6202,7 +6202,7 @@
       </c>
       <c r="E212" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6229,7 +6229,7 @@
       </c>
       <c r="E213" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6256,7 +6256,7 @@
       </c>
       <c r="E214" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6283,7 +6283,7 @@
       </c>
       <c r="E215" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6310,7 +6310,7 @@
       </c>
       <c r="E216" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6337,7 +6337,7 @@
       </c>
       <c r="E217" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6364,7 +6364,7 @@
       </c>
       <c r="E218" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6391,7 +6391,7 @@
       </c>
       <c r="E219" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6418,7 +6418,7 @@
       </c>
       <c r="E220" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6445,7 +6445,7 @@
       </c>
       <c r="E221" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6472,7 +6472,7 @@
       </c>
       <c r="E222" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6499,7 +6499,7 @@
       </c>
       <c r="E223" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6526,7 +6526,7 @@
       </c>
       <c r="E224" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6553,7 +6553,7 @@
       </c>
       <c r="E225" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6580,7 +6580,7 @@
       </c>
       <c r="E226" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6607,7 +6607,7 @@
       </c>
       <c r="E227" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6634,7 +6634,7 @@
       </c>
       <c r="E228" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6661,7 +6661,7 @@
       </c>
       <c r="E229" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6688,7 +6688,7 @@
       </c>
       <c r="E230" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6715,7 +6715,7 @@
       </c>
       <c r="E231" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6742,7 +6742,7 @@
       </c>
       <c r="E232" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6769,7 +6769,7 @@
       </c>
       <c r="E233" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6796,7 +6796,7 @@
       </c>
       <c r="E234" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6823,7 +6823,7 @@
       </c>
       <c r="E235" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6850,7 +6850,7 @@
       </c>
       <c r="E236" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6877,7 +6877,7 @@
       </c>
       <c r="E237" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6904,7 +6904,7 @@
       </c>
       <c r="E238" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6931,7 +6931,7 @@
       </c>
       <c r="E239" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6958,7 +6958,7 @@
       </c>
       <c r="E240" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -6985,7 +6985,7 @@
       </c>
       <c r="E241" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7012,7 +7012,7 @@
       </c>
       <c r="E242" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7039,7 +7039,7 @@
       </c>
       <c r="E243" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7066,7 +7066,7 @@
       </c>
       <c r="E244" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7093,7 +7093,7 @@
       </c>
       <c r="E245" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7120,7 +7120,7 @@
       </c>
       <c r="E246" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7147,7 +7147,7 @@
       </c>
       <c r="E247" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7174,7 +7174,7 @@
       </c>
       <c r="E248" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7201,7 +7201,7 @@
       </c>
       <c r="E249" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7228,7 +7228,7 @@
       </c>
       <c r="E250" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7255,7 +7255,7 @@
       </c>
       <c r="E251" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7282,7 +7282,7 @@
       </c>
       <c r="E252" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7309,7 +7309,7 @@
       </c>
       <c r="E253" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7336,7 +7336,7 @@
       </c>
       <c r="E254" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7363,7 +7363,7 @@
       </c>
       <c r="E255" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7390,7 +7390,7 @@
       </c>
       <c r="E256" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7417,7 +7417,7 @@
       </c>
       <c r="E257" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7444,7 +7444,7 @@
       </c>
       <c r="E258" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7471,7 +7471,7 @@
       </c>
       <c r="E259" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7498,7 +7498,7 @@
       </c>
       <c r="E260" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7525,7 +7525,7 @@
       </c>
       <c r="E261" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7552,7 +7552,7 @@
       </c>
       <c r="E262" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7579,7 +7579,7 @@
       </c>
       <c r="E263" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7606,7 +7606,7 @@
       </c>
       <c r="E264" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7633,7 +7633,7 @@
       </c>
       <c r="E265" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7660,7 +7660,7 @@
       </c>
       <c r="E266" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7687,7 +7687,7 @@
       </c>
       <c r="E267" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7714,7 +7714,7 @@
       </c>
       <c r="E268" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7741,7 +7741,7 @@
       </c>
       <c r="E269" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7768,7 +7768,7 @@
       </c>
       <c r="E270" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7795,7 +7795,7 @@
       </c>
       <c r="E271" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7822,7 +7822,7 @@
       </c>
       <c r="E272" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7849,7 +7849,7 @@
       </c>
       <c r="E273" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7876,7 +7876,7 @@
       </c>
       <c r="E274" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7903,7 +7903,7 @@
       </c>
       <c r="E275" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7930,7 +7930,7 @@
       </c>
       <c r="E276" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7957,7 +7957,7 @@
       </c>
       <c r="E277" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -7984,7 +7984,7 @@
       </c>
       <c r="E278" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -8011,7 +8011,7 @@
       </c>
       <c r="E279" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -8038,7 +8038,7 @@
       </c>
       <c r="E280" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -8065,7 +8065,7 @@
       </c>
       <c r="E281" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -8092,7 +8092,7 @@
       </c>
       <c r="E282" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -8119,7 +8119,7 @@
       </c>
       <c r="E283" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -8146,7 +8146,7 @@
       </c>
       <c r="E284" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -8173,7 +8173,7 @@
       </c>
       <c r="E285" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -8200,7 +8200,7 @@
       </c>
       <c r="E286" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -8227,7 +8227,7 @@
       </c>
       <c r="E287" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -8254,7 +8254,7 @@
       </c>
       <c r="E288" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -8281,7 +8281,7 @@
       </c>
       <c r="E289" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -8308,7 +8308,7 @@
       </c>
       <c r="E290" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -8335,7 +8335,7 @@
       </c>
       <c r="E291" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -8362,7 +8362,7 @@
       </c>
       <c r="E292" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -8389,7 +8389,7 @@
       </c>
       <c r="E293" s="4" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>
@@ -8416,7 +8416,7 @@
       </c>
       <c r="E294" s="3" t="inlineStr">
         <is>
-          <t>pediatrics trial reference file.xlsx</t>
+          <t>pediatrics trial reference file (1).xlsx</t>
         </is>
       </c>
     </row>

</xml_diff>